<commit_message>
Update Pharma Value-Based Measures Template.xlsx
</commit_message>
<xml_diff>
--- a/downloads/Pharma Value-Based Measures Template.xlsx
+++ b/downloads/Pharma Value-Based Measures Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="37280" windowHeight="18140" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="1120" yWindow="1960" windowWidth="37280" windowHeight="18140" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dropdown list" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1134,6 +1134,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1146,13 +1170,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1181,30 +1205,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="13" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2699,7 +2699,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2832,43 +2832,43 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="52" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="G14" s="55" t="s">
+      <c r="G14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="56"/>
-      <c r="I14" s="52" t="s">
+      <c r="H14" s="63"/>
+      <c r="I14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="J14" s="50" t="s">
+      <c r="J14" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="K14" s="52" t="s">
+      <c r="K14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="M14" s="55" t="s">
+      <c r="M14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="N14" s="56"/>
-      <c r="O14" s="52" t="s">
+      <c r="N14" s="63"/>
+      <c r="O14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="P14" s="50" t="s">
+      <c r="P14" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="Q14" s="52" t="s">
+      <c r="Q14" s="60" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2879,27 +2879,27 @@
       <c r="B15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="53"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="61"/>
       <c r="G15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I15" s="53"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="53"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="61"/>
       <c r="M15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="N15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="O15" s="53"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="53"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="61"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="35"/>
@@ -3124,7 +3124,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="P14:P15"/>
     <mergeCell ref="Q14:Q15"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I14:I15"/>
@@ -3136,6 +3135,7 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:C15"/>
+    <mergeCell ref="P14:P15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3362,10 +3362,10 @@
       <c r="A11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="51" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="33" t="s">
@@ -3374,10 +3374,10 @@
       <c r="G11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="69" t="s">
+      <c r="I11" s="53" t="s">
         <v>21</v>
       </c>
       <c r="J11" s="33" t="s">
@@ -3386,10 +3386,10 @@
       <c r="M11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="68" t="s">
+      <c r="N11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="69" t="s">
+      <c r="O11" s="53" t="s">
         <v>21</v>
       </c>
       <c r="P11" s="33" t="s">
@@ -3398,10 +3398,10 @@
       <c r="S11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="68" t="s">
+      <c r="T11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="U11" s="69" t="s">
+      <c r="U11" s="53" t="s">
         <v>21</v>
       </c>
       <c r="V11" s="33" t="s">
@@ -3410,10 +3410,10 @@
       <c r="Y11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="Z11" s="68" t="s">
+      <c r="Z11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AA11" s="69" t="s">
+      <c r="AA11" s="53" t="s">
         <v>21</v>
       </c>
       <c r="AB11" s="33" t="s">
@@ -3422,10 +3422,10 @@
       <c r="AE11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AF11" s="68" t="s">
+      <c r="AF11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AG11" s="69" t="s">
+      <c r="AG11" s="53" t="s">
         <v>21</v>
       </c>
       <c r="AH11" s="33" t="s">
@@ -3434,10 +3434,10 @@
       <c r="AK11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AL11" s="68" t="s">
+      <c r="AL11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AM11" s="69" t="s">
+      <c r="AM11" s="53" t="s">
         <v>21</v>
       </c>
       <c r="AN11" s="33" t="s">
@@ -3468,95 +3468,95 @@
       </c>
     </row>
     <row r="14" spans="1:41" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="52" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="G14" s="55" t="s">
+      <c r="G14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="56"/>
-      <c r="I14" s="52" t="s">
+      <c r="H14" s="63"/>
+      <c r="I14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="J14" s="50" t="s">
+      <c r="J14" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="K14" s="52" t="s">
+      <c r="K14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="M14" s="55" t="s">
+      <c r="M14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="N14" s="56"/>
-      <c r="O14" s="52" t="s">
+      <c r="N14" s="63"/>
+      <c r="O14" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="P14" s="50" t="s">
+      <c r="P14" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="Q14" s="52" t="s">
+      <c r="Q14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="S14" s="55" t="s">
+      <c r="S14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="T14" s="56"/>
-      <c r="U14" s="52" t="s">
+      <c r="T14" s="63"/>
+      <c r="U14" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="V14" s="50" t="s">
+      <c r="V14" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="W14" s="52" t="s">
+      <c r="W14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="Y14" s="55" t="s">
+      <c r="Y14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="Z14" s="56"/>
-      <c r="AA14" s="52" t="s">
+      <c r="Z14" s="63"/>
+      <c r="AA14" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="AB14" s="50" t="s">
+      <c r="AB14" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="AC14" s="52" t="s">
+      <c r="AC14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="AE14" s="55" t="s">
+      <c r="AE14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="AF14" s="56"/>
-      <c r="AG14" s="52" t="s">
+      <c r="AF14" s="63"/>
+      <c r="AG14" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="AH14" s="50" t="s">
+      <c r="AH14" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="AI14" s="52" t="s">
+      <c r="AI14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="AK14" s="55" t="s">
+      <c r="AK14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="AL14" s="56"/>
-      <c r="AM14" s="52" t="s">
+      <c r="AL14" s="63"/>
+      <c r="AM14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="AN14" s="50" t="s">
+      <c r="AN14" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="AO14" s="52" t="s">
+      <c r="AO14" s="60" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3567,63 +3567,63 @@
       <c r="B15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="53"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="61"/>
       <c r="G15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I15" s="53"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="53"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="61"/>
       <c r="M15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="N15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="O15" s="53"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="53"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="61"/>
       <c r="S15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="T15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="U15" s="53"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="53"/>
+      <c r="U15" s="61"/>
+      <c r="V15" s="59"/>
+      <c r="W15" s="61"/>
       <c r="Y15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="Z15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="AA15" s="53"/>
-      <c r="AB15" s="51"/>
-      <c r="AC15" s="53"/>
+      <c r="AA15" s="61"/>
+      <c r="AB15" s="59"/>
+      <c r="AC15" s="61"/>
       <c r="AE15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="AF15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="AG15" s="53"/>
-      <c r="AH15" s="51"/>
-      <c r="AI15" s="53"/>
+      <c r="AG15" s="61"/>
+      <c r="AH15" s="59"/>
+      <c r="AI15" s="61"/>
       <c r="AK15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="AL15" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="AM15" s="53"/>
-      <c r="AN15" s="51"/>
-      <c r="AO15" s="53"/>
+      <c r="AM15" s="61"/>
+      <c r="AN15" s="59"/>
+      <c r="AO15" s="61"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" s="47" t="s">
@@ -3635,7 +3635,7 @@
       <c r="C16" s="36">
         <v>0.96</v>
       </c>
-      <c r="D16" s="70">
+      <c r="D16" s="54">
         <v>0.2</v>
       </c>
       <c r="E16" s="35" t="s">
@@ -3647,10 +3647,10 @@
       <c r="H16" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="I16" s="70">
+      <c r="I16" s="54">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J16" s="71">
+      <c r="J16" s="55">
         <v>9.4E-2</v>
       </c>
       <c r="K16" s="35" t="str">
@@ -3663,10 +3663,10 @@
       <c r="N16" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="O16" s="72">
+      <c r="O16" s="56">
         <v>1300</v>
       </c>
-      <c r="P16" s="70">
+      <c r="P16" s="54">
         <v>0.37</v>
       </c>
       <c r="Q16" s="35" t="str">
@@ -3679,10 +3679,10 @@
       <c r="T16" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="U16" s="73">
+      <c r="U16" s="57">
         <v>32</v>
       </c>
-      <c r="V16" s="73">
+      <c r="V16" s="57">
         <v>7.6</v>
       </c>
       <c r="W16" s="35" t="str">
@@ -3695,10 +3695,10 @@
       <c r="Z16" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="AA16" s="73">
+      <c r="AA16" s="57">
         <v>65</v>
       </c>
-      <c r="AB16" s="73">
+      <c r="AB16" s="57">
         <v>12.3</v>
       </c>
       <c r="AC16" s="35" t="str">
@@ -3711,10 +3711,10 @@
       <c r="AF16" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="AG16" s="73">
+      <c r="AG16" s="57">
         <v>65</v>
       </c>
-      <c r="AH16" s="73">
+      <c r="AH16" s="57">
         <v>15.3</v>
       </c>
       <c r="AI16" s="35" t="str">
@@ -3727,10 +3727,10 @@
       <c r="AL16" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="AM16" s="73">
+      <c r="AM16" s="57">
         <v>10</v>
       </c>
-      <c r="AN16" s="73">
+      <c r="AN16" s="57">
         <v>1.3</v>
       </c>
       <c r="AO16" s="35" t="str">
@@ -3739,7 +3739,7 @@
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="64" t="s">
         <v>148</v>
       </c>
       <c r="B17" s="33" t="s">
@@ -3748,23 +3748,23 @@
       <c r="C17" s="36">
         <v>0.86292134831460676</v>
       </c>
-      <c r="D17" s="70">
+      <c r="D17" s="54">
         <v>0.18</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="G17" s="54" t="s">
+      <c r="G17" s="64" t="s">
         <v>148</v>
       </c>
       <c r="H17" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="I17" s="70">
+      <c r="I17" s="54">
         <f>0.5-C17/C$16*(0.5-I$16)</f>
         <v>0.30224719101123598</v>
       </c>
-      <c r="J17" s="71">
+      <c r="J17" s="55">
         <f>D17/D$16*J$16</f>
         <v>8.4599999999999995E-2</v>
       </c>
@@ -3772,17 +3772,17 @@
         <f t="shared" ref="K17:K29" si="3">ROUND(J17*100*0.8,1)&amp;" - "&amp;ROUND(J17*100*1.2,1)&amp;"%"</f>
         <v>6.8 - 10.2%</v>
       </c>
-      <c r="M17" s="54" t="s">
+      <c r="M17" s="64" t="s">
         <v>148</v>
       </c>
       <c r="N17" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="O17" s="72">
+      <c r="O17" s="56">
         <f>C17/C$16*O$16</f>
         <v>1168.5393258426968</v>
       </c>
-      <c r="P17" s="70">
+      <c r="P17" s="54">
         <f>D17/D$16*P$16</f>
         <v>0.33299999999999996</v>
       </c>
@@ -3790,17 +3790,17 @@
         <f t="shared" ref="Q17:Q29" si="4">ROUND(P17*100*0.9,0)&amp;" - "&amp;ROUND(P17*100*1.1,0)&amp;"%"</f>
         <v>30 - 37%</v>
       </c>
-      <c r="S17" s="54" t="s">
+      <c r="S17" s="64" t="s">
         <v>148</v>
       </c>
       <c r="T17" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="U17" s="73">
+      <c r="U17" s="57">
         <f>$C17/$C$16*U$16</f>
         <v>28.764044943820227</v>
       </c>
-      <c r="V17" s="73">
+      <c r="V17" s="57">
         <f>$D17/$D$16*V$16</f>
         <v>6.839999999999999</v>
       </c>
@@ -3808,17 +3808,17 @@
         <f t="shared" ref="W17:W29" si="5">ROUND(V17*0.9,1)&amp;" - "&amp;ROUND(V17*1.1,1)</f>
         <v>6.2 - 7.5</v>
       </c>
-      <c r="Y17" s="54" t="s">
+      <c r="Y17" s="64" t="s">
         <v>148</v>
       </c>
       <c r="Z17" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AA17" s="73">
+      <c r="AA17" s="57">
         <f>$C17/$C$16*AA$16</f>
         <v>58.426966292134836</v>
       </c>
-      <c r="AB17" s="73">
+      <c r="AB17" s="57">
         <f>$D17/$D$16*AB$16</f>
         <v>11.07</v>
       </c>
@@ -3826,17 +3826,17 @@
         <f t="shared" si="0"/>
         <v>10 - 12.2</v>
       </c>
-      <c r="AE17" s="54" t="s">
+      <c r="AE17" s="64" t="s">
         <v>148</v>
       </c>
       <c r="AF17" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AG17" s="73">
+      <c r="AG17" s="57">
         <f>$C17/$C$16*AG$16</f>
         <v>58.426966292134836</v>
       </c>
-      <c r="AH17" s="73">
+      <c r="AH17" s="57">
         <f>$D17/$D$16*AH$16</f>
         <v>13.77</v>
       </c>
@@ -3844,17 +3844,17 @@
         <f t="shared" si="1"/>
         <v>12.4 - 15.1</v>
       </c>
-      <c r="AK17" s="54" t="s">
+      <c r="AK17" s="64" t="s">
         <v>148</v>
       </c>
       <c r="AL17" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AM17" s="73">
+      <c r="AM17" s="57">
         <f>$C17/$C$16*AM$16</f>
         <v>8.9887640449438209</v>
       </c>
-      <c r="AN17" s="73">
+      <c r="AN17" s="57">
         <f>$D17/$D$16*AN$16</f>
         <v>1.17</v>
       </c>
@@ -3864,28 +3864,28 @@
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A18" s="54"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="33" t="s">
         <v>141</v>
       </c>
       <c r="C18" s="36">
         <v>1.0031460674157304</v>
       </c>
-      <c r="D18" s="70">
+      <c r="D18" s="54">
         <v>0.22</v>
       </c>
       <c r="E18" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="G18" s="54"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="I18" s="70">
+      <c r="I18" s="54">
         <f t="shared" ref="I18:I29" si="6">0.5-C18/C$16*(0.5-I$16)</f>
         <v>0.27011235955056179</v>
       </c>
-      <c r="J18" s="71">
+      <c r="J18" s="55">
         <f t="shared" ref="J18:J29" si="7">D18/D$16*J$16</f>
         <v>0.10339999999999999</v>
       </c>
@@ -3893,15 +3893,15 @@
         <f t="shared" si="3"/>
         <v>8.3 - 12.4%</v>
       </c>
-      <c r="M18" s="54"/>
+      <c r="M18" s="64"/>
       <c r="N18" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="O18" s="72">
+      <c r="O18" s="56">
         <f t="shared" ref="O18:P29" si="8">C18/C$16*O$16</f>
         <v>1358.4269662921349</v>
       </c>
-      <c r="P18" s="70">
+      <c r="P18" s="54">
         <f t="shared" si="8"/>
         <v>0.40699999999999997</v>
       </c>
@@ -3909,15 +3909,15 @@
         <f t="shared" si="4"/>
         <v>37 - 45%</v>
       </c>
-      <c r="S18" s="54"/>
+      <c r="S18" s="64"/>
       <c r="T18" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="U18" s="73">
+      <c r="U18" s="57">
         <f t="shared" ref="U18:V29" si="9">C18/C$16*U$16</f>
         <v>33.438202247191015</v>
       </c>
-      <c r="V18" s="73">
+      <c r="V18" s="57">
         <f t="shared" si="9"/>
         <v>8.36</v>
       </c>
@@ -3925,15 +3925,15 @@
         <f t="shared" si="5"/>
         <v>7.5 - 9.2</v>
       </c>
-      <c r="Y18" s="54"/>
+      <c r="Y18" s="64"/>
       <c r="Z18" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AA18" s="73">
+      <c r="AA18" s="57">
         <f t="shared" ref="AA18:AA29" si="10">$C18/$C$16*AA$16</f>
         <v>67.921348314606746</v>
       </c>
-      <c r="AB18" s="73">
+      <c r="AB18" s="57">
         <f t="shared" ref="AB18:AB29" si="11">$D18/$D$16*AB$16</f>
         <v>13.53</v>
       </c>
@@ -3941,15 +3941,15 @@
         <f t="shared" si="0"/>
         <v>12.2 - 14.9</v>
       </c>
-      <c r="AE18" s="54"/>
+      <c r="AE18" s="64"/>
       <c r="AF18" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AG18" s="73">
+      <c r="AG18" s="57">
         <f t="shared" ref="AG18:AG29" si="12">$C18/$C$16*AG$16</f>
         <v>67.921348314606746</v>
       </c>
-      <c r="AH18" s="73">
+      <c r="AH18" s="57">
         <f t="shared" ref="AH18:AH29" si="13">$D18/$D$16*AH$16</f>
         <v>16.829999999999998</v>
       </c>
@@ -3957,15 +3957,15 @@
         <f t="shared" si="1"/>
         <v>15.1 - 18.5</v>
       </c>
-      <c r="AK18" s="54"/>
+      <c r="AK18" s="64"/>
       <c r="AL18" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AM18" s="73">
+      <c r="AM18" s="57">
         <f t="shared" ref="AM18:AM29" si="14">$C18/$C$16*AM$16</f>
         <v>10.449438202247192</v>
       </c>
-      <c r="AN18" s="73">
+      <c r="AN18" s="57">
         <f t="shared" ref="AN18:AN29" si="15">$D18/$D$16*AN$16</f>
         <v>1.43</v>
       </c>
@@ -3975,7 +3975,7 @@
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="64" t="s">
         <v>149</v>
       </c>
       <c r="B19" s="33" t="s">
@@ -3984,23 +3984,23 @@
       <c r="C19" s="36">
         <v>0.97078651685393258</v>
       </c>
-      <c r="D19" s="70">
+      <c r="D19" s="54">
         <v>0.19</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="G19" s="54" t="s">
+      <c r="G19" s="64" t="s">
         <v>149</v>
       </c>
       <c r="H19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="I19" s="70">
+      <c r="I19" s="54">
         <f t="shared" si="6"/>
         <v>0.27752808988764044</v>
       </c>
-      <c r="J19" s="71">
+      <c r="J19" s="55">
         <f t="shared" si="7"/>
         <v>8.929999999999999E-2</v>
       </c>
@@ -4008,17 +4008,17 @@
         <f t="shared" si="3"/>
         <v>7.1 - 10.7%</v>
       </c>
-      <c r="M19" s="54" t="s">
+      <c r="M19" s="64" t="s">
         <v>149</v>
       </c>
       <c r="N19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="O19" s="72">
+      <c r="O19" s="56">
         <f t="shared" si="8"/>
         <v>1314.6067415730338</v>
       </c>
-      <c r="P19" s="70">
+      <c r="P19" s="54">
         <f t="shared" si="8"/>
         <v>0.35149999999999998</v>
       </c>
@@ -4026,17 +4026,17 @@
         <f t="shared" si="4"/>
         <v>32 - 39%</v>
       </c>
-      <c r="S19" s="54" t="s">
+      <c r="S19" s="64" t="s">
         <v>149</v>
       </c>
       <c r="T19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="U19" s="73">
+      <c r="U19" s="57">
         <f t="shared" si="9"/>
         <v>32.359550561797754</v>
       </c>
-      <c r="V19" s="73">
+      <c r="V19" s="57">
         <f t="shared" si="9"/>
         <v>7.22</v>
       </c>
@@ -4044,17 +4044,17 @@
         <f t="shared" si="5"/>
         <v>6.5 - 7.9</v>
       </c>
-      <c r="Y19" s="54" t="s">
+      <c r="Y19" s="64" t="s">
         <v>149</v>
       </c>
       <c r="Z19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AA19" s="73">
+      <c r="AA19" s="57">
         <f t="shared" si="10"/>
         <v>65.730337078651687</v>
       </c>
-      <c r="AB19" s="73">
+      <c r="AB19" s="57">
         <f t="shared" si="11"/>
         <v>11.685</v>
       </c>
@@ -4062,17 +4062,17 @@
         <f t="shared" si="0"/>
         <v>10.5 - 12.9</v>
       </c>
-      <c r="AE19" s="54" t="s">
+      <c r="AE19" s="64" t="s">
         <v>149</v>
       </c>
       <c r="AF19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AG19" s="73">
+      <c r="AG19" s="57">
         <f t="shared" si="12"/>
         <v>65.730337078651687</v>
       </c>
-      <c r="AH19" s="73">
+      <c r="AH19" s="57">
         <f t="shared" si="13"/>
         <v>14.535</v>
       </c>
@@ -4080,17 +4080,17 @@
         <f t="shared" si="1"/>
         <v>13.1 - 16</v>
       </c>
-      <c r="AK19" s="54" t="s">
+      <c r="AK19" s="64" t="s">
         <v>149</v>
       </c>
       <c r="AL19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AM19" s="73">
+      <c r="AM19" s="57">
         <f t="shared" si="14"/>
         <v>10.112359550561798</v>
       </c>
-      <c r="AN19" s="73">
+      <c r="AN19" s="57">
         <f t="shared" si="15"/>
         <v>1.2349999999999999</v>
       </c>
@@ -4100,28 +4100,28 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A20" s="54"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="33" t="s">
         <v>143</v>
       </c>
       <c r="C20" s="36">
         <v>0.94921348314606735</v>
       </c>
-      <c r="D20" s="70">
+      <c r="D20" s="54">
         <v>0.21</v>
       </c>
       <c r="E20" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="G20" s="54"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="I20" s="70">
+      <c r="I20" s="54">
         <f t="shared" si="6"/>
         <v>0.28247191011235961</v>
       </c>
-      <c r="J20" s="71">
+      <c r="J20" s="55">
         <f t="shared" si="7"/>
         <v>9.8699999999999982E-2</v>
       </c>
@@ -4129,15 +4129,15 @@
         <f t="shared" si="3"/>
         <v>7.9 - 11.8%</v>
       </c>
-      <c r="M20" s="54"/>
+      <c r="M20" s="64"/>
       <c r="N20" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="O20" s="72">
+      <c r="O20" s="56">
         <f t="shared" si="8"/>
         <v>1285.3932584269662</v>
       </c>
-      <c r="P20" s="70">
+      <c r="P20" s="54">
         <f t="shared" si="8"/>
         <v>0.38849999999999996</v>
       </c>
@@ -4145,15 +4145,15 @@
         <f t="shared" si="4"/>
         <v>35 - 43%</v>
       </c>
-      <c r="S20" s="54"/>
+      <c r="S20" s="64"/>
       <c r="T20" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="U20" s="73">
+      <c r="U20" s="57">
         <f t="shared" si="9"/>
         <v>31.640449438202246</v>
       </c>
-      <c r="V20" s="73">
+      <c r="V20" s="57">
         <f t="shared" si="9"/>
         <v>7.9799999999999986</v>
       </c>
@@ -4161,15 +4161,15 @@
         <f t="shared" si="5"/>
         <v>7.2 - 8.8</v>
       </c>
-      <c r="Y20" s="54"/>
+      <c r="Y20" s="64"/>
       <c r="Z20" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="AA20" s="73">
+      <c r="AA20" s="57">
         <f t="shared" si="10"/>
         <v>64.269662921348313</v>
       </c>
-      <c r="AB20" s="73">
+      <c r="AB20" s="57">
         <f t="shared" si="11"/>
         <v>12.914999999999999</v>
       </c>
@@ -4177,15 +4177,15 @@
         <f t="shared" si="0"/>
         <v>11.6 - 14.2</v>
       </c>
-      <c r="AE20" s="54"/>
+      <c r="AE20" s="64"/>
       <c r="AF20" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="AG20" s="73">
+      <c r="AG20" s="57">
         <f t="shared" si="12"/>
         <v>64.269662921348313</v>
       </c>
-      <c r="AH20" s="73">
+      <c r="AH20" s="57">
         <f t="shared" si="13"/>
         <v>16.064999999999998</v>
       </c>
@@ -4193,15 +4193,15 @@
         <f t="shared" si="1"/>
         <v>14.5 - 17.7</v>
       </c>
-      <c r="AK20" s="54"/>
+      <c r="AK20" s="64"/>
       <c r="AL20" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="AM20" s="73">
+      <c r="AM20" s="57">
         <f t="shared" si="14"/>
         <v>9.8876404494382015</v>
       </c>
-      <c r="AN20" s="73">
+      <c r="AN20" s="57">
         <f t="shared" si="15"/>
         <v>1.3649999999999998</v>
       </c>
@@ -4211,7 +4211,7 @@
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="64" t="s">
         <v>150</v>
       </c>
       <c r="B21" s="33" t="s">
@@ -4220,23 +4220,23 @@
       <c r="C21" s="36">
         <v>0.84134831460674153</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="54">
         <v>0.19</v>
       </c>
       <c r="E21" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="64" t="s">
         <v>150</v>
       </c>
       <c r="H21" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="I21" s="70">
+      <c r="I21" s="54">
         <f t="shared" si="6"/>
         <v>0.30719101123595505</v>
       </c>
-      <c r="J21" s="71">
+      <c r="J21" s="55">
         <f t="shared" si="7"/>
         <v>8.929999999999999E-2</v>
       </c>
@@ -4244,17 +4244,17 @@
         <f t="shared" si="3"/>
         <v>7.1 - 10.7%</v>
       </c>
-      <c r="M21" s="54" t="s">
+      <c r="M21" s="64" t="s">
         <v>150</v>
       </c>
       <c r="N21" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="O21" s="72">
+      <c r="O21" s="56">
         <f t="shared" si="8"/>
         <v>1139.3258426966293</v>
       </c>
-      <c r="P21" s="70">
+      <c r="P21" s="54">
         <f t="shared" si="8"/>
         <v>0.35149999999999998</v>
       </c>
@@ -4262,17 +4262,17 @@
         <f t="shared" si="4"/>
         <v>32 - 39%</v>
       </c>
-      <c r="S21" s="54" t="s">
+      <c r="S21" s="64" t="s">
         <v>150</v>
       </c>
       <c r="T21" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="U21" s="73">
+      <c r="U21" s="57">
         <f t="shared" si="9"/>
         <v>28.04494382022472</v>
       </c>
-      <c r="V21" s="73">
+      <c r="V21" s="57">
         <f t="shared" si="9"/>
         <v>7.22</v>
       </c>
@@ -4280,17 +4280,17 @@
         <f t="shared" si="5"/>
         <v>6.5 - 7.9</v>
       </c>
-      <c r="Y21" s="54" t="s">
+      <c r="Y21" s="64" t="s">
         <v>150</v>
       </c>
       <c r="Z21" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="AA21" s="73">
+      <c r="AA21" s="57">
         <f t="shared" si="10"/>
         <v>56.966292134831463</v>
       </c>
-      <c r="AB21" s="73">
+      <c r="AB21" s="57">
         <f t="shared" si="11"/>
         <v>11.685</v>
       </c>
@@ -4298,17 +4298,17 @@
         <f t="shared" si="0"/>
         <v>10.5 - 12.9</v>
       </c>
-      <c r="AE21" s="54" t="s">
+      <c r="AE21" s="64" t="s">
         <v>150</v>
       </c>
       <c r="AF21" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="AG21" s="73">
+      <c r="AG21" s="57">
         <f t="shared" si="12"/>
         <v>56.966292134831463</v>
       </c>
-      <c r="AH21" s="73">
+      <c r="AH21" s="57">
         <f t="shared" si="13"/>
         <v>14.535</v>
       </c>
@@ -4316,17 +4316,17 @@
         <f t="shared" si="1"/>
         <v>13.1 - 16</v>
       </c>
-      <c r="AK21" s="54" t="s">
+      <c r="AK21" s="64" t="s">
         <v>150</v>
       </c>
       <c r="AL21" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="AM21" s="73">
+      <c r="AM21" s="57">
         <f t="shared" si="14"/>
         <v>8.7640449438202257</v>
       </c>
-      <c r="AN21" s="73">
+      <c r="AN21" s="57">
         <f t="shared" si="15"/>
         <v>1.2349999999999999</v>
       </c>
@@ -4336,28 +4336,28 @@
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A22" s="54"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="33" t="s">
         <v>179</v>
       </c>
       <c r="C22" s="36">
         <v>1.0139325842696629</v>
       </c>
-      <c r="D22" s="70">
+      <c r="D22" s="54">
         <v>0.19</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="G22" s="54"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="I22" s="70">
+      <c r="I22" s="54">
         <f t="shared" si="6"/>
         <v>0.26764044943820225</v>
       </c>
-      <c r="J22" s="71">
+      <c r="J22" s="55">
         <f t="shared" si="7"/>
         <v>8.929999999999999E-2</v>
       </c>
@@ -4365,15 +4365,15 @@
         <f t="shared" si="3"/>
         <v>7.1 - 10.7%</v>
       </c>
-      <c r="M22" s="54"/>
+      <c r="M22" s="64"/>
       <c r="N22" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="O22" s="72">
+      <c r="O22" s="56">
         <f t="shared" si="8"/>
         <v>1373.0337078651687</v>
       </c>
-      <c r="P22" s="70">
+      <c r="P22" s="54">
         <f t="shared" si="8"/>
         <v>0.35149999999999998</v>
       </c>
@@ -4381,15 +4381,15 @@
         <f t="shared" si="4"/>
         <v>32 - 39%</v>
       </c>
-      <c r="S22" s="54"/>
+      <c r="S22" s="64"/>
       <c r="T22" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="U22" s="73">
+      <c r="U22" s="57">
         <f t="shared" si="9"/>
         <v>33.797752808988768</v>
       </c>
-      <c r="V22" s="73">
+      <c r="V22" s="57">
         <f t="shared" si="9"/>
         <v>7.22</v>
       </c>
@@ -4397,15 +4397,15 @@
         <f t="shared" si="5"/>
         <v>6.5 - 7.9</v>
       </c>
-      <c r="Y22" s="54"/>
+      <c r="Y22" s="64"/>
       <c r="Z22" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="AA22" s="73">
+      <c r="AA22" s="57">
         <f t="shared" si="10"/>
         <v>68.651685393258433</v>
       </c>
-      <c r="AB22" s="73">
+      <c r="AB22" s="57">
         <f t="shared" si="11"/>
         <v>11.685</v>
       </c>
@@ -4413,15 +4413,15 @@
         <f t="shared" si="0"/>
         <v>10.5 - 12.9</v>
       </c>
-      <c r="AE22" s="54"/>
+      <c r="AE22" s="64"/>
       <c r="AF22" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="AG22" s="73">
+      <c r="AG22" s="57">
         <f t="shared" si="12"/>
         <v>68.651685393258433</v>
       </c>
-      <c r="AH22" s="73">
+      <c r="AH22" s="57">
         <f t="shared" si="13"/>
         <v>14.535</v>
       </c>
@@ -4429,15 +4429,15 @@
         <f t="shared" si="1"/>
         <v>13.1 - 16</v>
       </c>
-      <c r="AK22" s="54"/>
+      <c r="AK22" s="64"/>
       <c r="AL22" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="AM22" s="73">
+      <c r="AM22" s="57">
         <f t="shared" si="14"/>
         <v>10.561797752808991</v>
       </c>
-      <c r="AN22" s="73">
+      <c r="AN22" s="57">
         <f t="shared" si="15"/>
         <v>1.2349999999999999</v>
       </c>
@@ -4447,28 +4447,28 @@
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A23" s="54"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="33" t="s">
         <v>180</v>
       </c>
       <c r="C23" s="36">
         <v>1.1865168539325843</v>
       </c>
-      <c r="D23" s="70">
+      <c r="D23" s="54">
         <v>0.25</v>
       </c>
       <c r="E23" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="G23" s="54"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="I23" s="70">
+      <c r="I23" s="54">
         <f t="shared" si="6"/>
         <v>0.22808988764044946</v>
       </c>
-      <c r="J23" s="71">
+      <c r="J23" s="55">
         <f t="shared" si="7"/>
         <v>0.11749999999999999</v>
       </c>
@@ -4476,30 +4476,30 @@
         <f t="shared" si="3"/>
         <v>9.4 - 14.1%</v>
       </c>
-      <c r="M23" s="54"/>
+      <c r="M23" s="64"/>
       <c r="N23" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="O23" s="72">
+      <c r="O23" s="56">
         <f t="shared" si="8"/>
         <v>1606.7415730337079</v>
       </c>
-      <c r="P23" s="70">
+      <c r="P23" s="54">
         <v>0.41</v>
       </c>
       <c r="Q23" s="35" t="str">
         <f t="shared" si="4"/>
         <v>37 - 45%</v>
       </c>
-      <c r="S23" s="54"/>
+      <c r="S23" s="64"/>
       <c r="T23" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="U23" s="73">
+      <c r="U23" s="57">
         <f t="shared" si="9"/>
         <v>39.550561797752813</v>
       </c>
-      <c r="V23" s="73">
+      <c r="V23" s="57">
         <f t="shared" si="9"/>
         <v>9.5</v>
       </c>
@@ -4507,15 +4507,15 @@
         <f t="shared" si="5"/>
         <v>8.6 - 10.5</v>
       </c>
-      <c r="Y23" s="54"/>
+      <c r="Y23" s="64"/>
       <c r="Z23" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="AA23" s="73">
+      <c r="AA23" s="57">
         <f t="shared" si="10"/>
         <v>80.337078651685403</v>
       </c>
-      <c r="AB23" s="73">
+      <c r="AB23" s="57">
         <f t="shared" si="11"/>
         <v>15.375</v>
       </c>
@@ -4523,15 +4523,15 @@
         <f t="shared" si="0"/>
         <v>13.8 - 16.9</v>
       </c>
-      <c r="AE23" s="54"/>
+      <c r="AE23" s="64"/>
       <c r="AF23" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="AG23" s="73">
+      <c r="AG23" s="57">
         <f t="shared" si="12"/>
         <v>80.337078651685403</v>
       </c>
-      <c r="AH23" s="73">
+      <c r="AH23" s="57">
         <f t="shared" si="13"/>
         <v>19.125</v>
       </c>
@@ -4539,15 +4539,15 @@
         <f t="shared" si="1"/>
         <v>17.2 - 21</v>
       </c>
-      <c r="AK23" s="54"/>
+      <c r="AK23" s="64"/>
       <c r="AL23" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="AM23" s="73">
+      <c r="AM23" s="57">
         <f t="shared" si="14"/>
         <v>12.359550561797754</v>
       </c>
-      <c r="AN23" s="73">
+      <c r="AN23" s="57">
         <f t="shared" si="15"/>
         <v>1.625</v>
       </c>
@@ -4557,7 +4557,7 @@
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="64" t="s">
         <v>151</v>
       </c>
       <c r="B24" s="33" t="s">
@@ -4566,23 +4566,23 @@
       <c r="C24" s="36">
         <v>0.73348314606741583</v>
       </c>
-      <c r="D24" s="70">
+      <c r="D24" s="54">
         <v>0.2</v>
       </c>
       <c r="E24" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="G24" s="54" t="s">
+      <c r="G24" s="64" t="s">
         <v>151</v>
       </c>
       <c r="H24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="I24" s="70">
+      <c r="I24" s="54">
         <f t="shared" si="6"/>
         <v>0.33191011235955059</v>
       </c>
-      <c r="J24" s="71">
+      <c r="J24" s="55">
         <f t="shared" si="7"/>
         <v>9.4E-2</v>
       </c>
@@ -4590,16 +4590,16 @@
         <f t="shared" si="3"/>
         <v>7.5 - 11.3%</v>
       </c>
-      <c r="M24" s="54" t="s">
+      <c r="M24" s="64" t="s">
         <v>151</v>
       </c>
       <c r="N24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="O24" s="72">
+      <c r="O24" s="56">
         <v>1200</v>
       </c>
-      <c r="P24" s="70">
+      <c r="P24" s="54">
         <f t="shared" si="8"/>
         <v>0.37</v>
       </c>
@@ -4607,17 +4607,17 @@
         <f t="shared" si="4"/>
         <v>33 - 41%</v>
       </c>
-      <c r="S24" s="54" t="s">
+      <c r="S24" s="64" t="s">
         <v>151</v>
       </c>
       <c r="T24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="U24" s="73">
+      <c r="U24" s="57">
         <f t="shared" si="9"/>
         <v>24.449438202247194</v>
       </c>
-      <c r="V24" s="73">
+      <c r="V24" s="57">
         <f t="shared" si="9"/>
         <v>7.6</v>
       </c>
@@ -4625,17 +4625,17 @@
         <f t="shared" si="5"/>
         <v>6.8 - 8.4</v>
       </c>
-      <c r="Y24" s="54" t="s">
+      <c r="Y24" s="64" t="s">
         <v>151</v>
       </c>
       <c r="Z24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AA24" s="73">
+      <c r="AA24" s="57">
         <f t="shared" si="10"/>
         <v>49.662921348314612</v>
       </c>
-      <c r="AB24" s="73">
+      <c r="AB24" s="57">
         <f t="shared" si="11"/>
         <v>12.3</v>
       </c>
@@ -4643,17 +4643,17 @@
         <f t="shared" si="0"/>
         <v>11.1 - 13.5</v>
       </c>
-      <c r="AE24" s="54" t="s">
+      <c r="AE24" s="64" t="s">
         <v>151</v>
       </c>
       <c r="AF24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AG24" s="73">
+      <c r="AG24" s="57">
         <f t="shared" si="12"/>
         <v>49.662921348314612</v>
       </c>
-      <c r="AH24" s="73">
+      <c r="AH24" s="57">
         <f t="shared" si="13"/>
         <v>15.3</v>
       </c>
@@ -4661,17 +4661,17 @@
         <f t="shared" si="1"/>
         <v>13.8 - 16.8</v>
       </c>
-      <c r="AK24" s="54" t="s">
+      <c r="AK24" s="64" t="s">
         <v>151</v>
       </c>
       <c r="AL24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AM24" s="73">
+      <c r="AM24" s="57">
         <f t="shared" si="14"/>
         <v>7.6404494382022481</v>
       </c>
-      <c r="AN24" s="73">
+      <c r="AN24" s="57">
         <f t="shared" si="15"/>
         <v>1.3</v>
       </c>
@@ -4681,28 +4681,28 @@
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A25" s="54"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="33" t="s">
         <v>145</v>
       </c>
       <c r="C25" s="36">
         <v>1.1757303370786518</v>
       </c>
-      <c r="D25" s="70">
+      <c r="D25" s="54">
         <v>0.2</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="G25" s="54"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="I25" s="70">
+      <c r="I25" s="54">
         <f t="shared" si="6"/>
         <v>0.23056179775280899</v>
       </c>
-      <c r="J25" s="71">
+      <c r="J25" s="55">
         <f t="shared" si="7"/>
         <v>9.4E-2</v>
       </c>
@@ -4710,15 +4710,15 @@
         <f t="shared" si="3"/>
         <v>7.5 - 11.3%</v>
       </c>
-      <c r="M25" s="54"/>
+      <c r="M25" s="64"/>
       <c r="N25" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="O25" s="72">
+      <c r="O25" s="56">
         <f t="shared" si="8"/>
         <v>1592.1348314606744</v>
       </c>
-      <c r="P25" s="70">
+      <c r="P25" s="54">
         <f t="shared" si="8"/>
         <v>0.37</v>
       </c>
@@ -4726,15 +4726,15 @@
         <f t="shared" si="4"/>
         <v>33 - 41%</v>
       </c>
-      <c r="S25" s="54"/>
+      <c r="S25" s="64"/>
       <c r="T25" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="U25" s="73">
+      <c r="U25" s="57">
         <f t="shared" si="9"/>
         <v>39.19101123595506</v>
       </c>
-      <c r="V25" s="73">
+      <c r="V25" s="57">
         <f t="shared" si="9"/>
         <v>7.6</v>
       </c>
@@ -4742,15 +4742,15 @@
         <f t="shared" si="5"/>
         <v>6.8 - 8.4</v>
       </c>
-      <c r="Y25" s="54"/>
+      <c r="Y25" s="64"/>
       <c r="Z25" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AA25" s="73">
+      <c r="AA25" s="57">
         <f t="shared" si="10"/>
         <v>79.606741573033716</v>
       </c>
-      <c r="AB25" s="73">
+      <c r="AB25" s="57">
         <f t="shared" si="11"/>
         <v>12.3</v>
       </c>
@@ -4758,15 +4758,15 @@
         <f t="shared" si="0"/>
         <v>11.1 - 13.5</v>
       </c>
-      <c r="AE25" s="54"/>
+      <c r="AE25" s="64"/>
       <c r="AF25" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AG25" s="73">
+      <c r="AG25" s="57">
         <f t="shared" si="12"/>
         <v>79.606741573033716</v>
       </c>
-      <c r="AH25" s="73">
+      <c r="AH25" s="57">
         <f t="shared" si="13"/>
         <v>15.3</v>
       </c>
@@ -4774,15 +4774,15 @@
         <f t="shared" si="1"/>
         <v>13.8 - 16.8</v>
       </c>
-      <c r="AK25" s="54"/>
+      <c r="AK25" s="64"/>
       <c r="AL25" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AM25" s="73">
+      <c r="AM25" s="57">
         <f t="shared" si="14"/>
         <v>12.247191011235955</v>
       </c>
-      <c r="AN25" s="73">
+      <c r="AN25" s="57">
         <f t="shared" si="15"/>
         <v>1.3</v>
       </c>
@@ -4792,7 +4792,7 @@
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="64" t="s">
         <v>152</v>
       </c>
       <c r="B26" s="33" t="s">
@@ -4801,23 +4801,23 @@
       <c r="C26" s="36">
         <v>0.94921348314606735</v>
       </c>
-      <c r="D26" s="70">
+      <c r="D26" s="54">
         <v>0.2</v>
       </c>
       <c r="E26" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="G26" s="54" t="s">
+      <c r="G26" s="64" t="s">
         <v>152</v>
       </c>
       <c r="H26" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="I26" s="70">
+      <c r="I26" s="54">
         <f t="shared" si="6"/>
         <v>0.28247191011235961</v>
       </c>
-      <c r="J26" s="71">
+      <c r="J26" s="55">
         <f t="shared" si="7"/>
         <v>9.4E-2</v>
       </c>
@@ -4825,17 +4825,17 @@
         <f t="shared" si="3"/>
         <v>7.5 - 11.3%</v>
       </c>
-      <c r="M26" s="54" t="s">
+      <c r="M26" s="64" t="s">
         <v>152</v>
       </c>
       <c r="N26" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="O26" s="72">
+      <c r="O26" s="56">
         <f t="shared" si="8"/>
         <v>1285.3932584269662</v>
       </c>
-      <c r="P26" s="70">
+      <c r="P26" s="54">
         <f t="shared" si="8"/>
         <v>0.37</v>
       </c>
@@ -4843,17 +4843,17 @@
         <f t="shared" si="4"/>
         <v>33 - 41%</v>
       </c>
-      <c r="S26" s="54" t="s">
+      <c r="S26" s="64" t="s">
         <v>152</v>
       </c>
       <c r="T26" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="U26" s="73">
+      <c r="U26" s="57">
         <f t="shared" si="9"/>
         <v>31.640449438202246</v>
       </c>
-      <c r="V26" s="73">
+      <c r="V26" s="57">
         <f t="shared" si="9"/>
         <v>7.6</v>
       </c>
@@ -4861,17 +4861,17 @@
         <f t="shared" si="5"/>
         <v>6.8 - 8.4</v>
       </c>
-      <c r="Y26" s="54" t="s">
+      <c r="Y26" s="64" t="s">
         <v>152</v>
       </c>
       <c r="Z26" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AA26" s="73">
+      <c r="AA26" s="57">
         <f t="shared" si="10"/>
         <v>64.269662921348313</v>
       </c>
-      <c r="AB26" s="73">
+      <c r="AB26" s="57">
         <f t="shared" si="11"/>
         <v>12.3</v>
       </c>
@@ -4879,17 +4879,17 @@
         <f t="shared" si="0"/>
         <v>11.1 - 13.5</v>
       </c>
-      <c r="AE26" s="54" t="s">
+      <c r="AE26" s="64" t="s">
         <v>152</v>
       </c>
       <c r="AF26" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AG26" s="73">
+      <c r="AG26" s="57">
         <f t="shared" si="12"/>
         <v>64.269662921348313</v>
       </c>
-      <c r="AH26" s="73">
+      <c r="AH26" s="57">
         <f t="shared" si="13"/>
         <v>15.3</v>
       </c>
@@ -4897,17 +4897,17 @@
         <f t="shared" si="1"/>
         <v>13.8 - 16.8</v>
       </c>
-      <c r="AK26" s="54" t="s">
+      <c r="AK26" s="64" t="s">
         <v>152</v>
       </c>
       <c r="AL26" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AM26" s="73">
+      <c r="AM26" s="57">
         <f t="shared" si="14"/>
         <v>9.8876404494382015</v>
       </c>
-      <c r="AN26" s="73">
+      <c r="AN26" s="57">
         <f t="shared" si="15"/>
         <v>1.3</v>
       </c>
@@ -4917,28 +4917,28 @@
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A27" s="54"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="33" t="s">
         <v>145</v>
       </c>
       <c r="C27" s="36">
         <v>0.98157303370786519</v>
       </c>
-      <c r="D27" s="70">
+      <c r="D27" s="54">
         <v>0.2</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="I27" s="70">
+      <c r="I27" s="54">
         <f t="shared" si="6"/>
         <v>0.27505617977528091</v>
       </c>
-      <c r="J27" s="71">
+      <c r="J27" s="55">
         <f t="shared" si="7"/>
         <v>9.4E-2</v>
       </c>
@@ -4946,15 +4946,15 @@
         <f t="shared" si="3"/>
         <v>7.5 - 11.3%</v>
       </c>
-      <c r="M27" s="54"/>
+      <c r="M27" s="64"/>
       <c r="N27" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="O27" s="72">
+      <c r="O27" s="56">
         <f t="shared" si="8"/>
         <v>1329.2134831460676</v>
       </c>
-      <c r="P27" s="70">
+      <c r="P27" s="54">
         <f t="shared" si="8"/>
         <v>0.37</v>
       </c>
@@ -4962,15 +4962,15 @@
         <f t="shared" si="4"/>
         <v>33 - 41%</v>
       </c>
-      <c r="S27" s="54"/>
+      <c r="S27" s="64"/>
       <c r="T27" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="U27" s="73">
+      <c r="U27" s="57">
         <f t="shared" si="9"/>
         <v>32.719101123595507</v>
       </c>
-      <c r="V27" s="73">
+      <c r="V27" s="57">
         <f t="shared" si="9"/>
         <v>7.6</v>
       </c>
@@ -4978,15 +4978,15 @@
         <f t="shared" si="5"/>
         <v>6.8 - 8.4</v>
       </c>
-      <c r="Y27" s="54"/>
+      <c r="Y27" s="64"/>
       <c r="Z27" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AA27" s="73">
+      <c r="AA27" s="57">
         <f t="shared" si="10"/>
         <v>66.460674157303373</v>
       </c>
-      <c r="AB27" s="73">
+      <c r="AB27" s="57">
         <f t="shared" si="11"/>
         <v>12.3</v>
       </c>
@@ -4994,15 +4994,15 @@
         <f t="shared" si="0"/>
         <v>11.1 - 13.5</v>
       </c>
-      <c r="AE27" s="54"/>
+      <c r="AE27" s="64"/>
       <c r="AF27" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AG27" s="73">
+      <c r="AG27" s="57">
         <f t="shared" si="12"/>
         <v>66.460674157303373</v>
       </c>
-      <c r="AH27" s="73">
+      <c r="AH27" s="57">
         <f t="shared" si="13"/>
         <v>15.3</v>
       </c>
@@ -5010,15 +5010,15 @@
         <f t="shared" si="1"/>
         <v>13.8 - 16.8</v>
       </c>
-      <c r="AK27" s="54"/>
+      <c r="AK27" s="64"/>
       <c r="AL27" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AM27" s="73">
+      <c r="AM27" s="57">
         <f t="shared" si="14"/>
         <v>10.224719101123597</v>
       </c>
-      <c r="AN27" s="73">
+      <c r="AN27" s="57">
         <f t="shared" si="15"/>
         <v>1.3</v>
       </c>
@@ -5028,7 +5028,7 @@
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="64" t="s">
         <v>153</v>
       </c>
       <c r="B28" s="33" t="s">
@@ -5037,23 +5037,23 @@
       <c r="C28" s="36">
         <v>0.75505617977528083</v>
       </c>
-      <c r="D28" s="70">
+      <c r="D28" s="54">
         <v>0.17</v>
       </c>
       <c r="E28" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="G28" s="54" t="s">
+      <c r="G28" s="64" t="s">
         <v>153</v>
       </c>
       <c r="H28" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="I28" s="70">
+      <c r="I28" s="54">
         <f t="shared" si="6"/>
         <v>0.32696629213483153</v>
       </c>
-      <c r="J28" s="71">
+      <c r="J28" s="55">
         <f t="shared" si="7"/>
         <v>7.9899999999999999E-2</v>
       </c>
@@ -5061,17 +5061,17 @@
         <f t="shared" si="3"/>
         <v>6.4 - 9.6%</v>
       </c>
-      <c r="M28" s="54" t="s">
+      <c r="M28" s="64" t="s">
         <v>153</v>
       </c>
       <c r="N28" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="O28" s="72">
+      <c r="O28" s="56">
         <f t="shared" si="8"/>
         <v>1022.4719101123594</v>
       </c>
-      <c r="P28" s="70">
+      <c r="P28" s="54">
         <f t="shared" si="8"/>
         <v>0.3145</v>
       </c>
@@ -5079,17 +5079,17 @@
         <f t="shared" si="4"/>
         <v>28 - 35%</v>
       </c>
-      <c r="S28" s="54" t="s">
+      <c r="S28" s="64" t="s">
         <v>153</v>
       </c>
       <c r="T28" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="U28" s="73">
+      <c r="U28" s="57">
         <f t="shared" si="9"/>
         <v>25.168539325842694</v>
       </c>
-      <c r="V28" s="73">
+      <c r="V28" s="57">
         <f t="shared" si="9"/>
         <v>6.46</v>
       </c>
@@ -5097,17 +5097,17 @@
         <f t="shared" si="5"/>
         <v>5.8 - 7.1</v>
       </c>
-      <c r="Y28" s="54" t="s">
+      <c r="Y28" s="64" t="s">
         <v>153</v>
       </c>
       <c r="Z28" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AA28" s="73">
+      <c r="AA28" s="57">
         <f t="shared" si="10"/>
         <v>51.123595505617971</v>
       </c>
-      <c r="AB28" s="73">
+      <c r="AB28" s="57">
         <f t="shared" si="11"/>
         <v>10.455</v>
       </c>
@@ -5115,17 +5115,17 @@
         <f t="shared" si="0"/>
         <v>9.4 - 11.5</v>
       </c>
-      <c r="AE28" s="54" t="s">
+      <c r="AE28" s="64" t="s">
         <v>153</v>
       </c>
       <c r="AF28" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AG28" s="73">
+      <c r="AG28" s="57">
         <f t="shared" si="12"/>
         <v>51.123595505617971</v>
       </c>
-      <c r="AH28" s="73">
+      <c r="AH28" s="57">
         <f t="shared" si="13"/>
         <v>13.005000000000001</v>
       </c>
@@ -5133,17 +5133,17 @@
         <f t="shared" si="1"/>
         <v>11.7 - 14.3</v>
       </c>
-      <c r="AK28" s="54" t="s">
+      <c r="AK28" s="64" t="s">
         <v>153</v>
       </c>
       <c r="AL28" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AM28" s="73">
+      <c r="AM28" s="57">
         <f t="shared" si="14"/>
         <v>7.8651685393258415</v>
       </c>
-      <c r="AN28" s="73">
+      <c r="AN28" s="57">
         <f t="shared" si="15"/>
         <v>1.105</v>
       </c>
@@ -5153,28 +5153,28 @@
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A29" s="54"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="33" t="s">
         <v>145</v>
       </c>
       <c r="C29" s="36">
         <v>1.1865168539325843</v>
       </c>
-      <c r="D29" s="70">
+      <c r="D29" s="54">
         <v>0.23</v>
       </c>
       <c r="E29" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="G29" s="54"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="I29" s="70">
+      <c r="I29" s="54">
         <f t="shared" si="6"/>
         <v>0.22808988764044946</v>
       </c>
-      <c r="J29" s="71">
+      <c r="J29" s="55">
         <f t="shared" si="7"/>
         <v>0.10809999999999999</v>
       </c>
@@ -5182,15 +5182,15 @@
         <f t="shared" si="3"/>
         <v>8.6 - 13%</v>
       </c>
-      <c r="M29" s="54"/>
+      <c r="M29" s="64"/>
       <c r="N29" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="O29" s="72">
+      <c r="O29" s="56">
         <f t="shared" si="8"/>
         <v>1606.7415730337079</v>
       </c>
-      <c r="P29" s="70">
+      <c r="P29" s="54">
         <f t="shared" si="8"/>
         <v>0.42549999999999999</v>
       </c>
@@ -5198,15 +5198,15 @@
         <f t="shared" si="4"/>
         <v>38 - 47%</v>
       </c>
-      <c r="S29" s="54"/>
+      <c r="S29" s="64"/>
       <c r="T29" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="U29" s="73">
+      <c r="U29" s="57">
         <f t="shared" si="9"/>
         <v>39.550561797752813</v>
       </c>
-      <c r="V29" s="73">
+      <c r="V29" s="57">
         <f t="shared" si="9"/>
         <v>8.7399999999999984</v>
       </c>
@@ -5214,15 +5214,15 @@
         <f t="shared" si="5"/>
         <v>7.9 - 9.6</v>
       </c>
-      <c r="Y29" s="54"/>
+      <c r="Y29" s="64"/>
       <c r="Z29" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AA29" s="73">
+      <c r="AA29" s="57">
         <f t="shared" si="10"/>
         <v>80.337078651685403</v>
       </c>
-      <c r="AB29" s="73">
+      <c r="AB29" s="57">
         <f t="shared" si="11"/>
         <v>14.145</v>
       </c>
@@ -5230,15 +5230,15 @@
         <f t="shared" si="0"/>
         <v>12.7 - 15.6</v>
       </c>
-      <c r="AE29" s="54"/>
+      <c r="AE29" s="64"/>
       <c r="AF29" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AG29" s="73">
+      <c r="AG29" s="57">
         <f t="shared" si="12"/>
         <v>80.337078651685403</v>
       </c>
-      <c r="AH29" s="73">
+      <c r="AH29" s="57">
         <f t="shared" si="13"/>
         <v>17.594999999999999</v>
       </c>
@@ -5246,15 +5246,15 @@
         <f t="shared" si="1"/>
         <v>15.8 - 19.4</v>
       </c>
-      <c r="AK29" s="54"/>
+      <c r="AK29" s="64"/>
       <c r="AL29" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AM29" s="73">
+      <c r="AM29" s="57">
         <f t="shared" si="14"/>
         <v>12.359550561797754</v>
       </c>
-      <c r="AN29" s="73">
+      <c r="AN29" s="57">
         <f t="shared" si="15"/>
         <v>1.4949999999999999</v>
       </c>
@@ -5317,11 +5317,6 @@
     <mergeCell ref="AG14:AG15"/>
     <mergeCell ref="AH14:AH15"/>
     <mergeCell ref="AI14:AI15"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="Y14:Z14"/>
     <mergeCell ref="AA14:AA15"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
@@ -5329,38 +5324,19 @@
     <mergeCell ref="O14:O15"/>
     <mergeCell ref="P14:P15"/>
     <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="I14:I15"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>INDIRECT(VLOOKUP(B11,'[1]Dropdown list'!#REF!,3,FALSE))</xm:f>
-          </x14:formula1>
-          <xm:sqref>I11 C11 O11 U11 AA11 AG11 AM11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>INDIRECT(VLOOKUP(A11,'[1]Dropdown list'!#REF!,3,FALSE))</xm:f>
-          </x14:formula1>
-          <xm:sqref>H11 B11 N11 T11 Z11 AF11 AL11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>INDIRECT('[1]Dropdown list'!#REF!)</xm:f>
-          </x14:formula1>
-          <xm:sqref>G11 A11 M11 S11 Y11 AE11 AK11</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5412,10 +5388,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="73" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -5432,9 +5408,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="62" t="s">
+      <c r="A5" s="68"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="70" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -5444,9 +5420,9 @@
       <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="62"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="14" t="s">
         <v>44</v>
       </c>
@@ -5458,8 +5434,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="57"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
@@ -5470,9 +5446,9 @@
       <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="62" t="s">
+      <c r="A8" s="68"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="70" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -5482,9 +5458,9 @@
       <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="60"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="62"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="14" t="s">
         <v>103</v>
       </c>
@@ -5496,8 +5472,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
-      <c r="B10" s="57" t="s">
+      <c r="A10" s="68"/>
+      <c r="B10" s="65" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -5514,8 +5490,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="60"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="13" t="s">
         <v>18</v>
       </c>
@@ -5530,8 +5506,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="60"/>
-      <c r="B12" s="57"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
@@ -5542,8 +5518,8 @@
       <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
-      <c r="B13" s="58"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="21" t="s">
         <v>20</v>
       </c>
@@ -5558,13 +5534,13 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="72" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -5578,9 +5554,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="62"/>
+      <c r="A15" s="68"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="14" t="s">
         <v>52</v>
       </c>
@@ -5588,9 +5564,9 @@
       <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="62"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="14" t="s">
         <v>53</v>
       </c>
@@ -5602,9 +5578,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="60"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="62"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="14" t="s">
         <v>54</v>
       </c>
@@ -5612,9 +5588,9 @@
       <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="62"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="14" t="s">
         <v>55</v>
       </c>
@@ -5622,8 +5598,8 @@
       <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="60"/>
-      <c r="B19" s="57"/>
+      <c r="A19" s="68"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="13" t="s">
         <v>22</v>
       </c>
@@ -5634,8 +5610,8 @@
       <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="60"/>
-      <c r="B20" s="57"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="13" t="s">
         <v>23</v>
       </c>
@@ -5646,9 +5622,9 @@
       <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="62" t="s">
+      <c r="A21" s="68"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="14" t="s">
@@ -5658,9 +5634,9 @@
       <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="62"/>
+      <c r="A22" s="68"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="14" t="s">
         <v>58</v>
       </c>
@@ -5672,9 +5648,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="62"/>
+      <c r="A23" s="68"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="14" t="s">
         <v>59</v>
       </c>
@@ -5682,8 +5658,8 @@
       <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
-      <c r="B24" s="57"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="13" t="s">
         <v>25</v>
       </c>
@@ -5698,9 +5674,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="62" t="s">
+      <c r="A25" s="68"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="70" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="14" t="s">
@@ -5710,9 +5686,9 @@
       <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="62"/>
+      <c r="A26" s="68"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="70"/>
       <c r="D26" s="14" t="s">
         <v>62</v>
       </c>
@@ -5720,9 +5696,9 @@
       <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="62"/>
+      <c r="A27" s="68"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="70"/>
       <c r="D27" s="14" t="s">
         <v>63</v>
       </c>
@@ -5730,9 +5706,9 @@
       <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="62" t="s">
+      <c r="A28" s="68"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="70" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="14" t="s">
@@ -5742,9 +5718,9 @@
       <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="62"/>
+      <c r="A29" s="68"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="14" t="s">
         <v>65</v>
       </c>
@@ -5752,9 +5728,9 @@
       <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="62" t="s">
+      <c r="A30" s="68"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="70" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="14" t="s">
@@ -5764,9 +5740,9 @@
       <c r="F30" s="20"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="60"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="62"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="70"/>
       <c r="D31" s="14" t="s">
         <v>67</v>
       </c>
@@ -5774,9 +5750,9 @@
       <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="60"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="62"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="70"/>
       <c r="D32" s="14" t="s">
         <v>68</v>
       </c>
@@ -5784,9 +5760,9 @@
       <c r="F32" s="20"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="60"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="62" t="s">
+      <c r="A33" s="68"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="70" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="14" t="s">
@@ -5800,9 +5776,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="62"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="70"/>
       <c r="D34" s="14" t="s">
         <v>70</v>
       </c>
@@ -5814,11 +5790,11 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="57" t="s">
+      <c r="A35" s="68"/>
+      <c r="B35" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="62" t="s">
+      <c r="C35" s="70" t="s">
         <v>30</v>
       </c>
       <c r="D35" s="14" t="s">
@@ -5828,9 +5804,9 @@
       <c r="F35" s="20"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="62"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="70"/>
       <c r="D36" s="14" t="s">
         <v>72</v>
       </c>
@@ -5838,9 +5814,9 @@
       <c r="F36" s="20"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="62" t="s">
+      <c r="A37" s="68"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="70" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="14" t="s">
@@ -5850,9 +5826,9 @@
       <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="63"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="71"/>
       <c r="D38" s="22" t="s">
         <v>74</v>
       </c>
@@ -5860,13 +5836,13 @@
       <c r="F38" s="24"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="59" t="s">
+      <c r="A39" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="C39" s="72" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="17" t="s">
@@ -5876,9 +5852,9 @@
       <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="60"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="62"/>
+      <c r="A40" s="68"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="70"/>
       <c r="D40" s="14" t="s">
         <v>76</v>
       </c>
@@ -5886,9 +5862,9 @@
       <c r="F40" s="20"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="57"/>
-      <c r="C41" s="62" t="s">
+      <c r="A41" s="68"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="70" t="s">
         <v>33</v>
       </c>
       <c r="D41" s="14" t="s">
@@ -5898,9 +5874,9 @@
       <c r="F41" s="20"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="60"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="62"/>
+      <c r="A42" s="68"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="70"/>
       <c r="D42" s="14" t="s">
         <v>78</v>
       </c>
@@ -5908,8 +5884,8 @@
       <c r="F42" s="20"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="60"/>
-      <c r="B43" s="57"/>
+      <c r="A43" s="68"/>
+      <c r="B43" s="65"/>
       <c r="C43" s="13" t="s">
         <v>34</v>
       </c>
@@ -5920,8 +5896,8 @@
       <c r="F43" s="20"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="60"/>
-      <c r="B44" s="57"/>
+      <c r="A44" s="68"/>
+      <c r="B44" s="65"/>
       <c r="C44" s="13" t="s">
         <v>35</v>
       </c>
@@ -5932,11 +5908,11 @@
       <c r="F44" s="20"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
-      <c r="B45" s="57" t="s">
+      <c r="A45" s="68"/>
+      <c r="B45" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="62" t="s">
+      <c r="C45" s="70" t="s">
         <v>36</v>
       </c>
       <c r="D45" s="14" t="s">
@@ -5946,9 +5922,9 @@
       <c r="F45" s="20"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="60"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="62"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="70"/>
       <c r="D46" s="14" t="s">
         <v>82</v>
       </c>
@@ -5956,9 +5932,9 @@
       <c r="F46" s="20"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="62" t="s">
+      <c r="A47" s="68"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="70" t="s">
         <v>37</v>
       </c>
       <c r="D47" s="14" t="s">
@@ -5968,9 +5944,9 @@
       <c r="F47" s="20"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="62"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="70"/>
       <c r="D48" s="14" t="s">
         <v>84</v>
       </c>
@@ -5978,9 +5954,9 @@
       <c r="F48" s="20"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="62"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="70"/>
       <c r="D49" s="14" t="s">
         <v>85</v>
       </c>
@@ -5988,8 +5964,8 @@
       <c r="F49" s="20"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="57"/>
+      <c r="A50" s="68"/>
+      <c r="B50" s="65"/>
       <c r="C50" s="13" t="s">
         <v>38</v>
       </c>
@@ -6000,8 +5976,8 @@
       <c r="F50" s="20"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="60"/>
-      <c r="B51" s="57"/>
+      <c r="A51" s="68"/>
+      <c r="B51" s="65"/>
       <c r="C51" s="13" t="s">
         <v>39</v>
       </c>
@@ -6016,8 +5992,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="57" t="s">
+      <c r="A52" s="68"/>
+      <c r="B52" s="65" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="13" t="s">
@@ -6030,8 +6006,8 @@
       <c r="F52" s="20"/>
     </row>
     <row r="53" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="61"/>
-      <c r="B53" s="58"/>
+      <c r="A53" s="69"/>
+      <c r="B53" s="66"/>
       <c r="C53" s="21" t="s">
         <v>41</v>
       </c>

</xml_diff>